<commit_message>
cleared bugs of tech and quiz rounds
</commit_message>
<xml_diff>
--- a/backend/data/690d645aa482c39ccb12daaa.xlsx
+++ b/backend/data/690d645aa482c39ccb12daaa.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -435,9 +435,20 @@
         <v>100</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Gagan Naik</v>
+      </c>
+      <c r="B4" t="str">
+        <v>mentalmilestone24@gmail.com</v>
+      </c>
+      <c r="C4">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>